<commit_message>
A* terminado, pero probado en pocos mapas
</commit_message>
<xml_diff>
--- a/mapfiles/template_mapsBLOCKS.xlsx
+++ b/mapfiles/template_mapsBLOCKS.xlsx
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM20" sqref="AM20:AM31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20:AJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,247 +459,247 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1">
         <v>15</v>
-      </c>
-      <c r="C1" s="1">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1">
-        <v>5</v>
-      </c>
-      <c r="M1" s="1">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1">
-        <v>3</v>
-      </c>
-      <c r="O1" s="1">
-        <v>2</v>
-      </c>
-      <c r="P1" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>0</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="U1" s="1">
+        <v>0</v>
+      </c>
+      <c r="V1" s="1">
+        <v>1</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2</v>
+      </c>
+      <c r="X1" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>10</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>11</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>13</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>14</v>
+      </c>
+      <c r="AJ1" s="1">
         <v>15</v>
-      </c>
-      <c r="V1" s="1">
-        <v>14</v>
-      </c>
-      <c r="W1" s="1">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>11</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>9</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>7</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>6</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>5</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>4</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>3</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>2</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="str">
         <f t="shared" ref="B2:B17" si="0">$A2  &amp; "," &amp; B$1</f>
-        <v>15,15</v>
+        <v>0,0</v>
       </c>
       <c r="C2" s="1" t="str">
         <f t="shared" ref="C2:Q17" si="1">$A2  &amp; "," &amp; C$1</f>
-        <v>15,14</v>
+        <v>0,1</v>
       </c>
       <c r="D2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,13</v>
+        <v>0,2</v>
       </c>
       <c r="E2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,12</v>
+        <v>0,3</v>
       </c>
       <c r="F2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,11</v>
+        <v>0,4</v>
       </c>
       <c r="G2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,10</v>
+        <v>0,5</v>
       </c>
       <c r="H2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,9</v>
+        <v>0,6</v>
       </c>
       <c r="I2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,8</v>
+        <v>0,7</v>
       </c>
       <c r="J2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,7</v>
+        <v>0,8</v>
       </c>
       <c r="K2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,6</v>
+        <v>0,9</v>
       </c>
       <c r="L2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,5</v>
+        <v>0,10</v>
       </c>
       <c r="M2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,4</v>
+        <v>0,11</v>
       </c>
       <c r="N2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,3</v>
+        <v>0,12</v>
       </c>
       <c r="O2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,2</v>
+        <v>0,13</v>
       </c>
       <c r="P2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,1</v>
+        <v>0,14</v>
       </c>
       <c r="Q2" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>15,0</v>
+        <v>0,15</v>
       </c>
       <c r="T2" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>14,15</v>
+        <v>1,0</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" ref="C3:P17" si="2">$A3  &amp; "," &amp; C$1</f>
-        <v>14,14</v>
+        <v>1,1</v>
       </c>
       <c r="D3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,13</v>
+        <v>1,2</v>
       </c>
       <c r="E3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,12</v>
+        <v>1,3</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,11</v>
+        <v>1,4</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,10</v>
+        <v>1,5</v>
       </c>
       <c r="H3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,9</v>
+        <v>1,6</v>
       </c>
       <c r="I3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,8</v>
+        <v>1,7</v>
       </c>
       <c r="J3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,7</v>
+        <v>1,8</v>
       </c>
       <c r="K3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,6</v>
+        <v>1,9</v>
       </c>
       <c r="L3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,5</v>
+        <v>1,10</v>
       </c>
       <c r="M3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,4</v>
+        <v>1,11</v>
       </c>
       <c r="N3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,3</v>
+        <v>1,12</v>
       </c>
       <c r="O3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,2</v>
+        <v>1,13</v>
       </c>
       <c r="P3" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>14,1</v>
+        <v>1,14</v>
       </c>
       <c r="Q3" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>14,0</v>
+        <v>1,15</v>
       </c>
       <c r="T3" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>6</v>
@@ -707,74 +707,74 @@
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>13,15</v>
+        <v>2,0</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,14</v>
+        <v>2,1</v>
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,13</v>
+        <v>2,2</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,12</v>
+        <v>2,3</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,11</v>
+        <v>2,4</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,10</v>
+        <v>2,5</v>
       </c>
       <c r="H4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,9</v>
+        <v>2,6</v>
       </c>
       <c r="I4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,8</v>
+        <v>2,7</v>
       </c>
       <c r="J4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,7</v>
+        <v>2,8</v>
       </c>
       <c r="K4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,6</v>
+        <v>2,9</v>
       </c>
       <c r="L4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,5</v>
+        <v>2,10</v>
       </c>
       <c r="M4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,4</v>
+        <v>2,11</v>
       </c>
       <c r="N4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,3</v>
+        <v>2,12</v>
       </c>
       <c r="O4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,2</v>
+        <v>2,13</v>
       </c>
       <c r="P4" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>13,1</v>
+        <v>2,14</v>
       </c>
       <c r="Q4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>13,0</v>
+        <v>2,15</v>
       </c>
       <c r="T4" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="AL4" s="3"/>
       <c r="AM4" s="3"/>
@@ -784,74 +784,74 @@
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>12,15</v>
+        <v>3,0</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,14</v>
+        <v>3,1</v>
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,13</v>
+        <v>3,2</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,12</v>
+        <v>3,3</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,11</v>
+        <v>3,4</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,10</v>
+        <v>3,5</v>
       </c>
       <c r="H5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,9</v>
+        <v>3,6</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,8</v>
+        <v>3,7</v>
       </c>
       <c r="J5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,7</v>
+        <v>3,8</v>
       </c>
       <c r="K5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,6</v>
+        <v>3,9</v>
       </c>
       <c r="L5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,5</v>
+        <v>3,10</v>
       </c>
       <c r="M5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,4</v>
+        <v>3,11</v>
       </c>
       <c r="N5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,3</v>
+        <v>3,12</v>
       </c>
       <c r="O5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,2</v>
+        <v>3,13</v>
       </c>
       <c r="P5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12,1</v>
+        <v>3,14</v>
       </c>
       <c r="Q5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>12,0</v>
+        <v>3,15</v>
       </c>
       <c r="T5" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="AL5" s="3"/>
       <c r="AM5" s="3"/>
@@ -861,74 +861,74 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>11,15</v>
+        <v>4,0</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,14</v>
+        <v>4,1</v>
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,13</v>
+        <v>4,2</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,12</v>
+        <v>4,3</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,11</v>
+        <v>4,4</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,10</v>
+        <v>4,5</v>
       </c>
       <c r="H6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,9</v>
+        <v>4,6</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,8</v>
+        <v>4,7</v>
       </c>
       <c r="J6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,7</v>
+        <v>4,8</v>
       </c>
       <c r="K6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,6</v>
+        <v>4,9</v>
       </c>
       <c r="L6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,5</v>
+        <v>4,10</v>
       </c>
       <c r="M6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,4</v>
+        <v>4,11</v>
       </c>
       <c r="N6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,3</v>
+        <v>4,12</v>
       </c>
       <c r="O6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,2</v>
+        <v>4,13</v>
       </c>
       <c r="P6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11,1</v>
+        <v>4,14</v>
       </c>
       <c r="Q6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>11,0</v>
+        <v>4,15</v>
       </c>
       <c r="T6" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
@@ -938,220 +938,220 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>10,15</v>
+        <v>5,0</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,14</v>
+        <v>5,1</v>
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,13</v>
+        <v>5,2</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,12</v>
+        <v>5,3</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,11</v>
+        <v>5,4</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,10</v>
+        <v>5,5</v>
       </c>
       <c r="H7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,9</v>
+        <v>5,6</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,8</v>
+        <v>5,7</v>
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,7</v>
+        <v>5,8</v>
       </c>
       <c r="K7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,6</v>
+        <v>5,9</v>
       </c>
       <c r="L7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,5</v>
+        <v>5,10</v>
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,4</v>
+        <v>5,11</v>
       </c>
       <c r="N7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,3</v>
+        <v>5,12</v>
       </c>
       <c r="O7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,2</v>
+        <v>5,13</v>
       </c>
       <c r="P7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10,1</v>
+        <v>5,14</v>
       </c>
       <c r="Q7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>10,0</v>
+        <v>5,15</v>
       </c>
       <c r="T7" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>9,15</v>
+        <v>6,0</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,14</v>
+        <v>6,1</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,13</v>
+        <v>6,2</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,12</v>
+        <v>6,3</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,11</v>
+        <v>6,4</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,10</v>
+        <v>6,5</v>
       </c>
       <c r="H8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,9</v>
+        <v>6,6</v>
       </c>
       <c r="I8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,8</v>
+        <v>6,7</v>
       </c>
       <c r="J8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,7</v>
+        <v>6,8</v>
       </c>
       <c r="K8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,6</v>
+        <v>6,9</v>
       </c>
       <c r="L8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,5</v>
+        <v>6,10</v>
       </c>
       <c r="M8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,4</v>
+        <v>6,11</v>
       </c>
       <c r="N8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,3</v>
+        <v>6,12</v>
       </c>
       <c r="O8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,2</v>
+        <v>6,13</v>
       </c>
       <c r="P8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9,1</v>
+        <v>6,14</v>
       </c>
       <c r="Q8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>9,0</v>
+        <v>6,15</v>
       </c>
       <c r="T8" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>8,15</v>
+        <v>7,0</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,14</v>
+        <v>7,1</v>
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,13</v>
+        <v>7,2</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,12</v>
+        <v>7,3</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,11</v>
+        <v>7,4</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,10</v>
+        <v>7,5</v>
       </c>
       <c r="H9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,9</v>
+        <v>7,6</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,8</v>
+        <v>7,7</v>
       </c>
       <c r="J9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,7</v>
+        <v>7,8</v>
       </c>
       <c r="K9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,6</v>
+        <v>7,9</v>
       </c>
       <c r="L9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,5</v>
+        <v>7,10</v>
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,4</v>
+        <v>7,11</v>
       </c>
       <c r="N9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,3</v>
+        <v>7,12</v>
       </c>
       <c r="O9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,2</v>
+        <v>7,13</v>
       </c>
       <c r="P9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8,1</v>
+        <v>7,14</v>
       </c>
       <c r="Q9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>8,0</v>
+        <v>7,15</v>
       </c>
       <c r="T9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AO9" s="1" t="s">
         <v>10</v>
@@ -1159,146 +1159,146 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>7,15</v>
+        <v>8,0</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,14</v>
+        <v>8,1</v>
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,13</v>
+        <v>8,2</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,12</v>
+        <v>8,3</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,11</v>
+        <v>8,4</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,10</v>
+        <v>8,5</v>
       </c>
       <c r="H10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,9</v>
+        <v>8,6</v>
       </c>
       <c r="I10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,8</v>
+        <v>8,7</v>
       </c>
       <c r="J10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,7</v>
+        <v>8,8</v>
       </c>
       <c r="K10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,6</v>
+        <v>8,9</v>
       </c>
       <c r="L10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,5</v>
+        <v>8,10</v>
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,4</v>
+        <v>8,11</v>
       </c>
       <c r="N10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,3</v>
+        <v>8,12</v>
       </c>
       <c r="O10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,2</v>
+        <v>8,13</v>
       </c>
       <c r="P10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7,1</v>
+        <v>8,14</v>
       </c>
       <c r="Q10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>7,0</v>
+        <v>8,15</v>
       </c>
       <c r="T10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>6,15</v>
+        <v>9,0</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,14</v>
+        <v>9,1</v>
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,13</v>
+        <v>9,2</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,12</v>
+        <v>9,3</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,11</v>
+        <v>9,4</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,10</v>
+        <v>9,5</v>
       </c>
       <c r="H11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,9</v>
+        <v>9,6</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,8</v>
+        <v>9,7</v>
       </c>
       <c r="J11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,7</v>
+        <v>9,8</v>
       </c>
       <c r="K11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,6</v>
+        <v>9,9</v>
       </c>
       <c r="L11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,5</v>
+        <v>9,10</v>
       </c>
       <c r="M11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,4</v>
+        <v>9,11</v>
       </c>
       <c r="N11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,3</v>
+        <v>9,12</v>
       </c>
       <c r="O11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,2</v>
+        <v>9,13</v>
       </c>
       <c r="P11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6,1</v>
+        <v>9,14</v>
       </c>
       <c r="Q11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>6,0</v>
+        <v>9,15</v>
       </c>
       <c r="T11" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AO11" s="1" t="s">
         <v>11</v>
@@ -1306,74 +1306,74 @@
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>5,15</v>
+        <v>10,0</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,14</v>
+        <v>10,1</v>
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,13</v>
+        <v>10,2</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,12</v>
+        <v>10,3</v>
       </c>
       <c r="F12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,11</v>
+        <v>10,4</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,10</v>
+        <v>10,5</v>
       </c>
       <c r="H12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,9</v>
+        <v>10,6</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,8</v>
+        <v>10,7</v>
       </c>
       <c r="J12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,7</v>
+        <v>10,8</v>
       </c>
       <c r="K12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,6</v>
+        <v>10,9</v>
       </c>
       <c r="L12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,5</v>
+        <v>10,10</v>
       </c>
       <c r="M12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,4</v>
+        <v>10,11</v>
       </c>
       <c r="N12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,3</v>
+        <v>10,12</v>
       </c>
       <c r="O12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,2</v>
+        <v>10,13</v>
       </c>
       <c r="P12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5,1</v>
+        <v>10,14</v>
       </c>
       <c r="Q12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>5,0</v>
+        <v>10,15</v>
       </c>
       <c r="T12" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AO12" s="1" t="s">
         <v>12</v>
@@ -1381,74 +1381,74 @@
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>4,15</v>
+        <v>11,0</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,14</v>
+        <v>11,1</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,13</v>
+        <v>11,2</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,12</v>
+        <v>11,3</v>
       </c>
       <c r="F13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,11</v>
+        <v>11,4</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,10</v>
+        <v>11,5</v>
       </c>
       <c r="H13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,9</v>
+        <v>11,6</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,8</v>
+        <v>11,7</v>
       </c>
       <c r="J13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,7</v>
+        <v>11,8</v>
       </c>
       <c r="K13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,6</v>
+        <v>11,9</v>
       </c>
       <c r="L13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,5</v>
+        <v>11,10</v>
       </c>
       <c r="M13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,4</v>
+        <v>11,11</v>
       </c>
       <c r="N13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,3</v>
+        <v>11,12</v>
       </c>
       <c r="O13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,2</v>
+        <v>11,13</v>
       </c>
       <c r="P13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4,1</v>
+        <v>11,14</v>
       </c>
       <c r="Q13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>4,0</v>
+        <v>11,15</v>
       </c>
       <c r="T13" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AO13" s="1" t="s">
         <v>13</v>
@@ -1456,74 +1456,74 @@
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>3,15</v>
+        <v>12,0</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,14</v>
+        <v>12,1</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,13</v>
+        <v>12,2</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,12</v>
+        <v>12,3</v>
       </c>
       <c r="F14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,11</v>
+        <v>12,4</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,10</v>
+        <v>12,5</v>
       </c>
       <c r="H14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,9</v>
+        <v>12,6</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,8</v>
+        <v>12,7</v>
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,7</v>
+        <v>12,8</v>
       </c>
       <c r="K14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,6</v>
+        <v>12,9</v>
       </c>
       <c r="L14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,5</v>
+        <v>12,10</v>
       </c>
       <c r="M14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,4</v>
+        <v>12,11</v>
       </c>
       <c r="N14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,3</v>
+        <v>12,12</v>
       </c>
       <c r="O14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,2</v>
+        <v>12,13</v>
       </c>
       <c r="P14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3,1</v>
+        <v>12,14</v>
       </c>
       <c r="Q14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3,0</v>
+        <v>12,15</v>
       </c>
       <c r="T14" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="AO14" s="1" t="s">
         <v>14</v>
@@ -1531,74 +1531,74 @@
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2,15</v>
+        <v>13,0</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,14</v>
+        <v>13,1</v>
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,13</v>
+        <v>13,2</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,12</v>
+        <v>13,3</v>
       </c>
       <c r="F15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,11</v>
+        <v>13,4</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,10</v>
+        <v>13,5</v>
       </c>
       <c r="H15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,9</v>
+        <v>13,6</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,8</v>
+        <v>13,7</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,7</v>
+        <v>13,8</v>
       </c>
       <c r="K15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,6</v>
+        <v>13,9</v>
       </c>
       <c r="L15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,5</v>
+        <v>13,10</v>
       </c>
       <c r="M15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,4</v>
+        <v>13,11</v>
       </c>
       <c r="N15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,3</v>
+        <v>13,12</v>
       </c>
       <c r="O15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,2</v>
+        <v>13,13</v>
       </c>
       <c r="P15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2,1</v>
+        <v>13,14</v>
       </c>
       <c r="Q15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2,0</v>
+        <v>13,15</v>
       </c>
       <c r="T15" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="AO15" s="1" t="s">
         <v>15</v>
@@ -1606,74 +1606,74 @@
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1,15</v>
+        <v>14,0</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,14</v>
+        <v>14,1</v>
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,13</v>
+        <v>14,2</v>
       </c>
       <c r="E16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,12</v>
+        <v>14,3</v>
       </c>
       <c r="F16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,11</v>
+        <v>14,4</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,10</v>
+        <v>14,5</v>
       </c>
       <c r="H16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,9</v>
+        <v>14,6</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,8</v>
+        <v>14,7</v>
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,7</v>
+        <v>14,8</v>
       </c>
       <c r="K16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,6</v>
+        <v>14,9</v>
       </c>
       <c r="L16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,5</v>
+        <v>14,10</v>
       </c>
       <c r="M16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,4</v>
+        <v>14,11</v>
       </c>
       <c r="N16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,3</v>
+        <v>14,12</v>
       </c>
       <c r="O16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,2</v>
+        <v>14,13</v>
       </c>
       <c r="P16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1,1</v>
+        <v>14,14</v>
       </c>
       <c r="Q16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1,0</v>
+        <v>14,15</v>
       </c>
       <c r="T16" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="AO16" s="1" t="s">
         <v>16</v>
@@ -1681,74 +1681,74 @@
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0,15</v>
+        <v>15,0</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,14</v>
+        <v>15,1</v>
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,13</v>
+        <v>15,2</v>
       </c>
       <c r="E17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,12</v>
+        <v>15,3</v>
       </c>
       <c r="F17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,11</v>
+        <v>15,4</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,10</v>
+        <v>15,5</v>
       </c>
       <c r="H17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,9</v>
+        <v>15,6</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,8</v>
+        <v>15,7</v>
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,7</v>
+        <v>15,8</v>
       </c>
       <c r="K17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,6</v>
+        <v>15,9</v>
       </c>
       <c r="L17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,5</v>
+        <v>15,10</v>
       </c>
       <c r="M17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,4</v>
+        <v>15,11</v>
       </c>
       <c r="N17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,3</v>
+        <v>15,12</v>
       </c>
       <c r="O17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,2</v>
+        <v>15,13</v>
       </c>
       <c r="P17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0,1</v>
+        <v>15,14</v>
       </c>
       <c r="Q17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>0,0</v>
+        <v>15,15</v>
       </c>
       <c r="T17" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
@@ -1766,100 +1766,100 @@
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>6</v>
+      </c>
+      <c r="I20" s="1">
+        <v>7</v>
+      </c>
+      <c r="J20" s="1">
+        <v>8</v>
+      </c>
+      <c r="K20" s="1">
+        <v>9</v>
+      </c>
+      <c r="L20" s="1">
+        <v>10</v>
+      </c>
+      <c r="M20" s="1">
+        <v>11</v>
+      </c>
+      <c r="N20" s="1">
+        <v>12</v>
+      </c>
+      <c r="O20" s="1">
+        <v>13</v>
+      </c>
+      <c r="P20" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q20" s="1">
         <v>15</v>
       </c>
-      <c r="C20" s="1">
+      <c r="U20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1">
+        <v>1</v>
+      </c>
+      <c r="W20" s="1">
+        <v>2</v>
+      </c>
+      <c r="X20" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>8</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>9</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>10</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>11</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>13</v>
+      </c>
+      <c r="AI20" s="1">
         <v>14</v>
       </c>
-      <c r="D20" s="1">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1">
-        <v>11</v>
-      </c>
-      <c r="G20" s="1">
-        <v>10</v>
-      </c>
-      <c r="H20" s="1">
-        <v>9</v>
-      </c>
-      <c r="I20" s="1">
-        <v>8</v>
-      </c>
-      <c r="J20" s="1">
-        <v>7</v>
-      </c>
-      <c r="K20" s="1">
-        <v>6</v>
-      </c>
-      <c r="L20" s="1">
-        <v>5</v>
-      </c>
-      <c r="M20" s="1">
-        <v>4</v>
-      </c>
-      <c r="N20" s="1">
-        <v>3</v>
-      </c>
-      <c r="O20" s="1">
-        <v>2</v>
-      </c>
-      <c r="P20" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>0</v>
-      </c>
-      <c r="U20" s="1">
+      <c r="AJ20" s="1">
         <v>15</v>
-      </c>
-      <c r="V20" s="1">
-        <v>14</v>
-      </c>
-      <c r="W20" s="1">
-        <v>13</v>
-      </c>
-      <c r="X20" s="1">
-        <v>12</v>
-      </c>
-      <c r="Y20" s="1">
-        <v>11</v>
-      </c>
-      <c r="Z20" s="1">
-        <v>10</v>
-      </c>
-      <c r="AA20" s="1">
-        <v>9</v>
-      </c>
-      <c r="AB20" s="1">
-        <v>8</v>
-      </c>
-      <c r="AC20" s="1">
-        <v>7</v>
-      </c>
-      <c r="AD20" s="1">
-        <v>6</v>
-      </c>
-      <c r="AE20" s="1">
-        <v>5</v>
-      </c>
-      <c r="AF20" s="1">
-        <v>4</v>
-      </c>
-      <c r="AG20" s="1">
-        <v>3</v>
-      </c>
-      <c r="AH20" s="1">
-        <v>2</v>
-      </c>
-      <c r="AI20" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ20" s="1">
-        <v>0</v>
       </c>
       <c r="AM20" s="1" t="s">
         <v>4</v>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T21" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="U21" s="1" t="str">
         <f>IF(B21="","",CONCATENATE(B2,";",B21))</f>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="T22" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="U22" s="1" t="str">
         <f t="shared" ref="U22:U36" si="4">IF(B22="","",CONCATENATE(B3,";",B22))</f>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
@@ -2029,7 +2029,7 @@
         <v>3</v>
       </c>
       <c r="T23" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="U23" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="X23" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>13,12;2</v>
+        <v>2,3;2</v>
       </c>
       <c r="Y23" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="AF23" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>13,4;3</v>
+        <v>2,11;3</v>
       </c>
       <c r="AG23" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="AH23" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>13,2;3</v>
+        <v>2,13;3</v>
       </c>
       <c r="AI23" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2101,10 +2101,10 @@
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="T24" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="U24" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="N25" s="1">
         <v>3</v>
       </c>
       <c r="T25" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="U25" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="AG25" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>11,3;3</v>
+        <v>4,12;3</v>
       </c>
       <c r="AH25" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T26" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="U26" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2329,10 +2329,10 @@
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="T27" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="U27" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2404,10 +2404,10 @@
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T28" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U28" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2479,10 +2479,10 @@
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T29" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U29" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H30" s="1">
         <v>1</v>
@@ -2572,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="T30" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="U30" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2600,23 +2600,23 @@
       </c>
       <c r="AA30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6,9;1</v>
+        <v>9,6;1</v>
       </c>
       <c r="AB30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6,8;1</v>
+        <v>9,7;1</v>
       </c>
       <c r="AC30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6,7;1</v>
+        <v>9,8;1</v>
       </c>
       <c r="AD30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6,6;1</v>
+        <v>9,9;1</v>
       </c>
       <c r="AE30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6,5;1</v>
+        <v>9,10;1</v>
       </c>
       <c r="AF30" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2644,13 +2644,13 @@
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H31" s="1">
         <v>1</v>
       </c>
       <c r="T31" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U31" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="AA31" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>5,9;1</v>
+        <v>10,6;1</v>
       </c>
       <c r="AB31" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H32" s="1">
         <v>1</v>
       </c>
       <c r="T32" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="U32" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="AA32" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>4,9;1</v>
+        <v>11,6;1</v>
       </c>
       <c r="AB32" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2798,13 +2798,13 @@
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H33" s="1">
         <v>1</v>
       </c>
       <c r="T33" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="U33" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="AA33" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>3,9;1</v>
+        <v>12,6;1</v>
       </c>
       <c r="AB33" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2874,10 +2874,10 @@
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="T34" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="U34" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2947,10 +2947,10 @@
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="T35" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="U35" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3020,10 +3020,10 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T36" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U36" s="1" t="str">
         <f t="shared" si="4"/>

</xml_diff>